<commit_message>
Added better support for testing the Kpi new import formats
</commit_message>
<xml_diff>
--- a/public/sample_uploads/kpi_extraction/MIS Sample2.xlsx
+++ b/public/sample_uploads/kpi_extraction/MIS Sample2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\kpi_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78F2FB2-26E6-4E0C-B3E0-AFF68EAD4B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979C9CBF-64ED-44A3-9223-76BD5D7CA74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="2" xr2:uid="{43C73447-205B-4618-8EF2-F374A5CFCAEF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
   <si>
     <t>Revenue from Operations</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Net Profit after tax</t>
+  </si>
+  <si>
+    <t>Q4FY22</t>
   </si>
 </sst>
 </file>
@@ -598,7 +601,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -613,7 +616,9 @@
       <c r="C1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7"/>
+      <c r="D1" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="E1" s="7" t="s">
         <v>13</v>
       </c>
@@ -631,6 +636,9 @@
       <c r="C2" s="1">
         <v>13017</v>
       </c>
+      <c r="D2" s="1">
+        <v>13017</v>
+      </c>
       <c r="E2" s="1">
         <v>63856</v>
       </c>
@@ -648,6 +656,9 @@
       <c r="C3" s="1">
         <v>5758</v>
       </c>
+      <c r="D3" s="1">
+        <v>5758</v>
+      </c>
       <c r="E3" s="1">
         <v>27392</v>
       </c>
@@ -665,6 +676,9 @@
       <c r="C4" s="2">
         <v>0.442</v>
       </c>
+      <c r="D4" s="2">
+        <v>0.442</v>
+      </c>
       <c r="E4" s="2">
         <v>0.42899999999999999</v>
       </c>
@@ -682,6 +696,9 @@
       <c r="C5">
         <v>707</v>
       </c>
+      <c r="D5">
+        <v>707</v>
+      </c>
       <c r="E5" s="1">
         <v>3462</v>
       </c>
@@ -699,6 +716,9 @@
       <c r="C6" s="2">
         <v>5.3999999999999999E-2</v>
       </c>
+      <c r="D6" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
       <c r="E6" s="2">
         <v>5.3999999999999999E-2</v>
       </c>
@@ -716,6 +736,9 @@
       <c r="C7">
         <v>86</v>
       </c>
+      <c r="D7">
+        <v>86</v>
+      </c>
       <c r="E7">
         <v>690</v>
       </c>
@@ -733,6 +756,9 @@
       <c r="C8" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
+      <c r="D8" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
       <c r="E8" s="2">
         <v>1.0999999999999999E-2</v>
       </c>
@@ -750,6 +776,9 @@
       <c r="C9">
         <v>23</v>
       </c>
+      <c r="D9">
+        <v>23</v>
+      </c>
       <c r="E9">
         <v>397</v>
       </c>
@@ -767,6 +796,9 @@
       <c r="C10" s="2">
         <v>2E-3</v>
       </c>
+      <c r="D10" s="2">
+        <v>2E-3</v>
+      </c>
       <c r="E10" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -784,6 +816,9 @@
       <c r="C11">
         <v>721</v>
       </c>
+      <c r="D11">
+        <v>721</v>
+      </c>
       <c r="E11" s="1">
         <v>3807</v>
       </c>
@@ -799,6 +834,9 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="C12" s="2">
+        <v>5.5E-2</v>
+      </c>
+      <c r="D12" s="2">
         <v>5.5E-2</v>
       </c>
       <c r="E12" s="2">
@@ -1426,10 +1464,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3A9A8F-1CA1-4269-A601-EEA18B3504D2}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="E11" sqref="E11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1437,7 +1475,7 @@
     <col min="1" max="1" width="39.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1447,8 +1485,17 @@
       <c r="C1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1458,8 +1505,17 @@
       <c r="C2" s="1">
         <v>7297</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E2" s="1">
+        <v>6979</v>
+      </c>
+      <c r="F2" s="1">
+        <v>7297</v>
+      </c>
+      <c r="G2" s="1">
+        <v>7297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1469,8 +1525,17 @@
       <c r="C3" s="1">
         <v>9033</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E3" s="1">
+        <v>10499</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9033</v>
+      </c>
+      <c r="G3" s="1">
+        <v>9033</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1480,8 +1545,17 @@
       <c r="C4" s="1">
         <v>16330</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E4" s="1">
+        <v>17478</v>
+      </c>
+      <c r="F4" s="1">
+        <v>16330</v>
+      </c>
+      <c r="G4" s="1">
+        <v>16330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1491,8 +1565,17 @@
       <c r="C5" s="1">
         <v>13922</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E5" s="1">
+        <v>12810</v>
+      </c>
+      <c r="F5" s="1">
+        <v>13922</v>
+      </c>
+      <c r="G5" s="1">
+        <v>13922</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1502,8 +1585,17 @@
       <c r="C6" s="1">
         <v>1515</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E6" s="1">
+        <v>4159</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1515</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1513,8 +1605,17 @@
       <c r="C7">
         <v>893</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E7">
+        <v>510</v>
+      </c>
+      <c r="F7">
+        <v>893</v>
+      </c>
+      <c r="G7">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1524,8 +1625,17 @@
       <c r="C8" s="1">
         <v>16330</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E8" s="1">
+        <v>17478</v>
+      </c>
+      <c r="F8" s="1">
+        <v>16330</v>
+      </c>
+      <c r="G8" s="1">
+        <v>16330</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
@@ -1535,8 +1645,17 @@
       <c r="C11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1546,8 +1665,17 @@
       <c r="C12">
         <v>278</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E12">
+        <v>337</v>
+      </c>
+      <c r="F12">
+        <v>278</v>
+      </c>
+      <c r="G12">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1557,8 +1685,17 @@
       <c r="C13" s="1">
         <v>-1169</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E13" s="1">
+        <v>-1479</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-1169</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-1169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1568,8 +1705,17 @@
       <c r="C14" s="1">
         <v>1670</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E14" s="1">
+        <v>2320</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1670</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1579,8 +1725,17 @@
       <c r="C15" s="1">
         <v>-4395</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E15" s="1">
+        <v>-4130</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-4395</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-4395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1590,8 +1745,17 @@
       <c r="C16" s="1">
         <v>-2784</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E16" s="1">
+        <v>-1107</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-2784</v>
+      </c>
+      <c r="G16" s="1">
+        <v>-2784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1601,8 +1765,17 @@
       <c r="C17" s="1">
         <v>1552</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E17" s="1">
+        <v>2476</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1552</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1610,6 +1783,15 @@
         <v>-443</v>
       </c>
       <c r="C18" s="1">
+        <v>-3957</v>
+      </c>
+      <c r="E18">
+        <v>-443</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-3957</v>
+      </c>
+      <c r="G18" s="1">
         <v>-3957</v>
       </c>
     </row>

</xml_diff>